<commit_message>
Added functions to HomePage
</commit_message>
<xml_diff>
--- a/testautomation/src/main/resources/SourceDataFiles/ClientData.xlsx
+++ b/testautomation/src/main/resources/SourceDataFiles/ClientData.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+  <si>
+    <t xml:space="preserve">IdClient</t>
+  </si>
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -43,6 +46,12 @@
     <t xml:space="preserve">BornDate</t>
   </si>
   <si>
+    <t xml:space="preserve">NationalId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1001</t>
+  </si>
+  <si>
     <t xml:space="preserve">Enrique</t>
   </si>
   <si>
@@ -55,10 +64,16 @@
     <t xml:space="preserve">10/10/1980</t>
   </si>
   <si>
+    <t xml:space="preserve">C1002</t>
+  </si>
+  <si>
     <t xml:space="preserve">Edgar</t>
   </si>
   <si>
-    <t xml:space="preserve">lizcarrillo119999@gmail.com</t>
+    <t xml:space="preserve">edgarcarrillo119999@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1003</t>
   </si>
   <si>
     <t xml:space="preserve">Myriam</t>
@@ -67,10 +82,13 @@
     <t xml:space="preserve">myriamcarrillo119999@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Liz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">edgarcarrillo119999@gmail.com</t>
+    <t xml:space="preserve">C1004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Julio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">juliocarrillo119999@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -81,7 +99,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -102,12 +120,20 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Consolas"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -159,12 +185,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -172,7 +206,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -193,188 +227,173 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.07"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="38.07"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="5" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.32"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1011" min="10" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1012" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>8</v>
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>33443344</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>3344334433</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
+      <c r="H2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>447711</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>33443344</v>
       </c>
-      <c r="F3" s="0" t="n">
-        <v>3344334433</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
+      <c r="G3" s="1" t="n">
+        <v>3344334444</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>447712</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>33443344</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>3344334455</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>33443344</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>3344334433</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>10</v>
+      <c r="I4" s="1" t="n">
+        <v>447713</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="0" t="n">
+      <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <v>33443344</v>
       </c>
-      <c r="F5" s="0" t="n">
-        <v>3344334433</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G21" s="2"/>
+      <c r="G5" s="1" t="n">
+        <v>3344334466</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>447714</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="enriquecarrillo119999@gmail.com"/>
-    <hyperlink ref="C3" r:id="rId2" display="lizcarrillo119999@gmail.com"/>
-    <hyperlink ref="C4" r:id="rId3" display="myriamcarrillo119999@gmail.com"/>
-    <hyperlink ref="C5" r:id="rId4" display="edgarcarrillo119999@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId1" display="enriquecarrillo119999@gmail.com"/>
+    <hyperlink ref="D3" r:id="rId2" display="edgarcarrillo119999@gmail.com"/>
+    <hyperlink ref="D4" r:id="rId3" display="myriamcarrillo119999@gmail.com"/>
+    <hyperlink ref="D5" r:id="rId4" display="juliocarrillo119999@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Rename FrameworkConfig to FWConfig, added excel files to SourceDataFiles folder.
</commit_message>
<xml_diff>
--- a/testautomation/src/main/resources/SourceDataFiles/ClientData.xlsx
+++ b/testautomation/src/main/resources/SourceDataFiles/ClientData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t xml:space="preserve">IdClient</t>
   </si>
@@ -31,6 +31,9 @@
     <t xml:space="preserve">LastName</t>
   </si>
   <si>
+    <t xml:space="preserve">Gender</t>
+  </si>
+  <si>
     <t xml:space="preserve">Email</t>
   </si>
   <si>
@@ -58,6 +61,9 @@
     <t xml:space="preserve">Carrillo</t>
   </si>
   <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
     <t xml:space="preserve">enriquecarrillo119999@gmail.com</t>
   </si>
   <si>
@@ -77,6 +83,9 @@
   </si>
   <si>
     <t xml:space="preserve">Myriam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
   </si>
   <si>
     <t xml:space="preserve">myriamcarrillo119999@gmail.com</t>
@@ -227,20 +236,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="38.07"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="5" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.32"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1011" min="10" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1012" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="38.07"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="6" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.32"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1009" min="11" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1010" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -271,129 +281,144 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="G2" s="1" t="n">
         <v>33443344</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="H2" s="1" t="n">
         <v>3344334433</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="1" t="n">
+      <c r="I2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="1" t="n">
         <v>447711</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>33443344</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>3344334444</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>33443344</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>3344334444</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="1" t="n">
+      <c r="J3" s="1" t="n">
         <v>447712</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="G4" s="1" t="n">
         <v>33443344</v>
       </c>
-      <c r="G4" s="1" t="n">
+      <c r="H4" s="1" t="n">
         <v>3344334455</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="1" t="n">
+      <c r="I4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="1" t="n">
         <v>447713</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="F5" s="1" t="n">
+      <c r="G5" s="1" t="n">
         <v>33443344</v>
       </c>
-      <c r="G5" s="1" t="n">
+      <c r="H5" s="1" t="n">
         <v>3344334466</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="1" t="n">
+      <c r="I5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="1" t="n">
         <v>447714</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="enriquecarrillo119999@gmail.com"/>
-    <hyperlink ref="D3" r:id="rId2" display="edgarcarrillo119999@gmail.com"/>
-    <hyperlink ref="D4" r:id="rId3" display="myriamcarrillo119999@gmail.com"/>
-    <hyperlink ref="D5" r:id="rId4" display="juliocarrillo119999@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId1" display="enriquecarrillo119999@gmail.com"/>
+    <hyperlink ref="E3" r:id="rId2" display="edgarcarrillo119999@gmail.com"/>
+    <hyperlink ref="E4" r:id="rId3" display="myriamcarrillo119999@gmail.com"/>
+    <hyperlink ref="E5" r:id="rId4" display="juliocarrillo119999@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>